<commit_message>
FIX: Fix slotType list, complete te_spreadsheet_template
</commit_message>
<xml_diff>
--- a/module/admin-api/InitFiles/te_spreadsheet_template.xlsx
+++ b/module/admin-api/InitFiles/te_spreadsheet_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="-5540" windowWidth="27960" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="29640" yWindow="-5540" windowWidth="27960" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="触发意图" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>信息名称</t>
   </si>
@@ -108,13 +108,85 @@
   </si>
   <si>
     <t>请至少填入一句话术。</t>
+  </si>
+  <si>
+    <t>时间日期</t>
+  </si>
+  <si>
+    <t>时间日期(粒度-分)(未来时间)</t>
+  </si>
+  <si>
+    <t>时间日期(粒度-天)(未来时间)</t>
+  </si>
+  <si>
+    <t>人数</t>
+  </si>
+  <si>
+    <t>来电人姓氏</t>
+  </si>
+  <si>
+    <t>联络人姓氏</t>
+  </si>
+  <si>
+    <t>电子邮件</t>
+  </si>
+  <si>
+    <t>大陆手机号码</t>
+  </si>
+  <si>
+    <t>大陆固定电话号码+手机号码</t>
+  </si>
+  <si>
+    <t>台湾固定电话号码+手机号码</t>
+  </si>
+  <si>
+    <t>是否</t>
+  </si>
+  <si>
+    <t>车牌号码</t>
+  </si>
+  <si>
+    <t>包厢还是大堂</t>
+  </si>
+  <si>
+    <t>宝宝椅</t>
+  </si>
+  <si>
+    <t>是否排号</t>
+  </si>
+  <si>
+    <t>特殊需求</t>
+  </si>
+  <si>
+    <t>信用卡号</t>
+  </si>
+  <si>
+    <t>金钱</t>
+  </si>
+  <si>
+    <t>金融实体类别</t>
+  </si>
+  <si>
+    <t>餐饮实体类别</t>
+  </si>
+  <si>
+    <t>注意</t>
+  </si>
+  <si>
+    <t>请勿更改Sheet Name</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>说明</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,8 +194,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +247,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,11 +278,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -566,69 +691,210 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="62.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="5"/>
+      <c r="E20" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="3"/>
+      <c r="E22" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>